<commit_message>
Login Details Updated changes
</commit_message>
<xml_diff>
--- a/src/main/java/com/BhimanaGroup/testData/BhimanGroup.xlsx
+++ b/src/main/java/com/BhimanaGroup/testData/BhimanGroup.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>UserName</t>
   </si>
@@ -399,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -422,15 +422,15 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2">
-        <v>9876543211</v>
+        <v>987654321</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="2">
-        <v>987654321</v>
+      <c r="A3" t="s">
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -438,7 +438,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -446,7 +446,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -454,84 +454,76 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>6</v>
+      <c r="A7" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="B8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2">
+      <c r="A9" s="2">
+        <v>9876543211</v>
+      </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2">
         <v>9876543211</v>
       </c>
-      <c r="B10" t="s">
-        <v>8</v>
+      <c r="B10">
+        <v>123456789</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="2">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="2">
         <v>9876543211</v>
       </c>
-      <c r="B11">
-        <v>123456789</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="2"/>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2">
         <v>9876543211</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>11</v>
+      <c r="B13" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2">
         <v>9876543211</v>
       </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2">
-        <v>9876543211</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="2">
         <v>987654211</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B15" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A8" r:id="rId1"/>
+    <hyperlink ref="A7" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes in excel file path
</commit_message>
<xml_diff>
--- a/src/main/java/com/BhimanaGroup/testData/BhimanGroup.xlsx
+++ b/src/main/java/com/BhimanaGroup/testData/BhimanGroup.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>UserName</t>
   </si>
@@ -399,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -422,15 +422,15 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2">
+        <v>9876543211</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2">
         <v>987654321</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -438,7 +438,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -446,7 +446,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -454,76 +454,84 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
       <c r="B8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="2">
-        <v>9876543211</v>
-      </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2">
         <v>9876543211</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="2">
+        <v>9876543211</v>
+      </c>
+      <c r="B11">
         <v>123456789</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="2"/>
-    </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="2">
-        <v>9876543211</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A12" s="2"/>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2">
         <v>9876543211</v>
       </c>
-      <c r="B13" t="s">
-        <v>10</v>
+      <c r="B13" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2">
         <v>9876543211</v>
       </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2">
+        <v>9876543211</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="2">
         <v>987654211</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A7" r:id="rId1"/>
+    <hyperlink ref="A8" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modification in login page
</commit_message>
<xml_diff>
--- a/src/main/java/com/BhimanaGroup/testData/BhimanGroup.xlsx
+++ b/src/main/java/com/BhimanaGroup/testData/BhimanGroup.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\urbanLadder\BhimanGroup\src\main\java\com\BhimanaGroup\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="192" yWindow="60" windowWidth="19092" windowHeight="9504"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>UserName</t>
   </si>
@@ -57,8 +62,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +116,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -157,7 +170,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -189,9 +202,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -223,6 +237,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -398,21 +413,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -420,142 +435,137 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
+        <v>987654321</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <v>9876543211</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2">
-        <v>987654321</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
       <c r="B9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9876543211</v>
       </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="2">
+      <c r="B10">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
         <v>9876543211</v>
       </c>
-      <c r="B11">
-        <v>123456789</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="2"/>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>9876543211</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>9876543211</v>
       </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
-        <v>9876543211</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="2">
         <v>987654211</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B15" t="s">
         <v>9</v>
       </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A8" r:id="rId1"/>
+    <hyperlink ref="A7" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changes in login page
</commit_message>
<xml_diff>
--- a/src/main/java/com/BhimanaGroup/testData/BhimanGroup.xlsx
+++ b/src/main/java/com/BhimanaGroup/testData/BhimanGroup.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="masterTap" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>UserName</t>
   </si>
@@ -52,6 +52,30 @@
   </si>
   <si>
     <t xml:space="preserve">    admin</t>
+  </si>
+  <si>
+    <t>Banks</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>Branches</t>
+  </si>
+  <si>
+    <t>Customers</t>
+  </si>
+  <si>
+    <t>Brokers</t>
+  </si>
+  <si>
+    <t>Vendors</t>
+  </si>
+  <si>
+    <t>Enquiry</t>
+  </si>
+  <si>
+    <t>Projects</t>
   </si>
 </sst>
 </file>
@@ -401,9 +425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -531,13 +553,60 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Final changes in login page and login test
</commit_message>
<xml_diff>
--- a/src/main/java/com/BhimanaGroup/testData/BhimanGroup.xlsx
+++ b/src/main/java/com/BhimanaGroup/testData/BhimanGroup.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>UserName</t>
   </si>
@@ -32,51 +32,23 @@
     <t>admin</t>
   </si>
   <si>
-    <t>Ashwini</t>
+    <t>admin12</t>
   </si>
   <si>
-    <t>ashwin1336</t>
-  </si>
-  <si>
-    <t>12345ashu</t>
-  </si>
-  <si>
-    <t>9876_543211admin</t>
-  </si>
-  <si>
-    <t>987654321@</t>
-  </si>
-  <si>
-    <t>adm</t>
-  </si>
-  <si>
-    <t>ashwini</t>
-  </si>
-  <si>
-    <t>_admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    admin</t>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -96,22 +68,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -414,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -436,7 +402,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>987654321</v>
       </c>
       <c r="B2" t="s">
@@ -444,105 +410,43 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>9876543211</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>9876543211</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
+      <c r="A7" s="1">
+        <v>99865845367</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>9876543211</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>9876543211</v>
-      </c>
-      <c r="B10">
-        <v>123456789</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>9876543211</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>9876543211</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>9876543211</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>987654211</v>
-      </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A7" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
master page framework design
</commit_message>
<xml_diff>
--- a/src/main/java/com/BhimanaGroup/testData/BhimanGroup.xlsx
+++ b/src/main/java/com/BhimanaGroup/testData/BhimanGroup.xlsx
@@ -1,19 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\urbanLadder\BhimanGroup\src\main\java\com\BhimanaGroup\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="192" yWindow="60" windowWidth="19092" windowHeight="9504"/>
+    <workbookView xWindow="192" yWindow="60" windowWidth="19092" windowHeight="9504" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="masterFunction" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>UserName</t>
   </si>
@@ -36,13 +31,40 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Bank</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Branches</t>
+  </si>
+  <si>
+    <t>Customers</t>
+  </si>
+  <si>
+    <t>Brokers</t>
+  </si>
+  <si>
+    <t>Vendors</t>
+  </si>
+  <si>
+    <t>Enquiry</t>
+  </si>
+  <si>
+    <t>Projects</t>
+  </si>
+  <si>
+    <t>masterTab</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,7 +158,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -168,10 +190,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -203,7 +224,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -379,21 +399,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -401,7 +421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="1">
         <v>987654321</v>
       </c>
@@ -409,7 +429,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -417,7 +437,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" s="1">
         <v>9876543211</v>
       </c>
@@ -425,7 +445,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="1">
         <v>9876543211</v>
       </c>
@@ -433,12 +453,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="B6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" s="1">
         <v>99865845367</v>
       </c>
@@ -452,24 +472,73 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Master module is perfectly done
</commit_message>
<xml_diff>
--- a/src/main/java/com/BhimanaGroup/testData/BhimanGroup.xlsx
+++ b/src/main/java/com/BhimanaGroup/testData/BhimanGroup.xlsx
@@ -1,14 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\urbanLadder\BhimanGroup\src\main\java\com\BhimanaGroup\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="192" yWindow="60" windowWidth="19092" windowHeight="9504" activeTab="1"/>
+    <workbookView xWindow="192" yWindow="60" windowWidth="19092" windowHeight="9504"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
-    <sheet name="masterFunction" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>UserName</t>
   </si>
@@ -32,39 +37,12 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
-  <si>
-    <t>Bank</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>Branches</t>
-  </si>
-  <si>
-    <t>Customers</t>
-  </si>
-  <si>
-    <t>Brokers</t>
-  </si>
-  <si>
-    <t>Vendors</t>
-  </si>
-  <si>
-    <t>Enquiry</t>
-  </si>
-  <si>
-    <t>Projects</t>
-  </si>
-  <si>
-    <t>masterTab</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,7 +136,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -190,9 +168,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -224,6 +203,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -399,21 +379,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -421,7 +401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>987654321</v>
       </c>
@@ -429,7 +409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -437,7 +417,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>9876543211</v>
       </c>
@@ -445,7 +425,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>9876543211</v>
       </c>
@@ -453,12 +433,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>99865845367</v>
       </c>
@@ -472,73 +452,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Screen shot taken in Users page module
</commit_message>
<xml_diff>
--- a/src/main/java/com/BhimanaGroup/testData/BhimanGroup.xlsx
+++ b/src/main/java/com/BhimanaGroup/testData/BhimanGroup.xlsx
@@ -1,19 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\urbanLadder\BhimanGroup\src\main\java\com\BhimanaGroup\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="192" yWindow="60" windowWidth="19092" windowHeight="9504"/>
+    <workbookView xWindow="192" yWindow="60" windowWidth="19092" windowHeight="9504" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="UsersDetails" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="48">
   <si>
     <t>UserName</t>
   </si>
@@ -36,19 +31,155 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>EmailId</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>JoiningDate</t>
+  </si>
+  <si>
+    <t>MobileNumber</t>
+  </si>
+  <si>
+    <t>BloodGroup</t>
+  </si>
+  <si>
+    <t>BankName</t>
+  </si>
+  <si>
+    <t>AccountNumber</t>
+  </si>
+  <si>
+    <t>IFSCCode</t>
+  </si>
+  <si>
+    <t>Resume</t>
+  </si>
+  <si>
+    <t>Agreement</t>
+  </si>
+  <si>
+    <t>KYC</t>
+  </si>
+  <si>
+    <t>FatherName</t>
+  </si>
+  <si>
+    <t>FatherOccupation</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>Priynka</t>
+  </si>
+  <si>
+    <t>P@gmail.com</t>
+  </si>
+  <si>
+    <t>B positive</t>
+  </si>
+  <si>
+    <t>JalGavBank</t>
+  </si>
+  <si>
+    <t>Khushal</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>bholenath</t>
+  </si>
+  <si>
+    <t>n@gmail.com</t>
+  </si>
+  <si>
+    <t>s@gmail.com</t>
+  </si>
+  <si>
+    <t>a@gmail.com</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>narayan</t>
+  </si>
+  <si>
+    <t>baliram</t>
+  </si>
+  <si>
+    <t>JJSB0000033</t>
+  </si>
+  <si>
+    <t>doctor</t>
+  </si>
+  <si>
+    <t>police</t>
+  </si>
+  <si>
+    <t>Sucheta</t>
+  </si>
+  <si>
+    <t>C:\\Users\\Lenovo\\Desktop\\Resume_Ashwini.pdf</t>
+  </si>
+  <si>
+    <t>MobileNumber1</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Bhushan</t>
+  </si>
+  <si>
+    <t>Broker1</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>sonale</t>
+  </si>
+  <si>
+    <t>Nagesh</t>
+  </si>
+  <si>
+    <t>JJSB0000034</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -68,16 +199,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -136,7 +274,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -168,10 +306,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -203,7 +340,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -379,21 +515,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -401,7 +537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="1">
         <v>987654321</v>
       </c>
@@ -409,7 +545,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -417,7 +553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" s="1">
         <v>9876543211</v>
       </c>
@@ -425,7 +561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="1">
         <v>9876543211</v>
       </c>
@@ -433,12 +569,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="B6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" s="1">
         <v>99865845367</v>
       </c>
@@ -452,26 +588,388 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24" customWidth="1"/>
+    <col min="11" max="11" width="24.21875" customWidth="1"/>
+    <col min="12" max="12" width="20" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2">
+        <v>9212121212</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="3">
+        <v>43862</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2">
+        <v>1010101011</v>
+      </c>
+      <c r="I2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2">
+        <v>9988776655</v>
+      </c>
+      <c r="O2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3">
+        <v>9323232323</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="3">
+        <v>43863</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3">
+        <v>1010101011</v>
+      </c>
+      <c r="I3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3">
+        <v>9988776655</v>
+      </c>
+      <c r="O3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4">
+        <v>6434343434</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="3">
+        <v>43864</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4">
+        <v>1010101011</v>
+      </c>
+      <c r="I4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4">
+        <v>9988776655</v>
+      </c>
+      <c r="O4" t="s">
+        <v>37</v>
+      </c>
+      <c r="P4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5">
+        <v>9545454545</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="3">
+        <v>43865</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5">
+        <v>1010101011</v>
+      </c>
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5">
+        <v>9988776655</v>
+      </c>
+      <c r="O5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>28</v>
+      </c>
+      <c r="R5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6">
+        <v>7766885544</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="3">
+        <v>43866</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6">
+        <v>1010101012</v>
+      </c>
+      <c r="I6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6">
+        <v>9988776656</v>
+      </c>
+      <c r="O6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>28</v>
+      </c>
+      <c r="R6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C5" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>